<commit_message>
webAutomation 增加数据库，增加物理按钮，点击cssid cssname 输入 cssid cssname
</commit_message>
<xml_diff>
--- a/ApplicationPerformance/webautomation/webfunctioncase.xlsx
+++ b/ApplicationPerformance/webautomation/webfunctioncase.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="13680" yWindow="1160" windowWidth="24300" windowHeight="14940" tabRatio="500"/>
+    <workbookView xWindow="2260" yWindow="2900" windowWidth="24300" windowHeight="14940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="browseefuncase" sheetId="5" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="153">
   <si>
     <t>用例编号</t>
     <rPh sb="0" eb="1">
@@ -575,10 +575,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -652,10 +648,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Yes</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>No</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -667,6 +659,173 @@
     <rPh sb="2" eb="3">
       <t>an'n</t>
     </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击_tagname</t>
+    <rPh sb="0" eb="1">
+      <t>dian'ji</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>点击_cssname</t>
+    <rPh sb="0" eb="1">
+      <t>dian'ji</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>tj_trnews</t>
+  </si>
+  <si>
+    <t>点击_cssid</t>
+    <rPh sb="0" eb="1">
+      <t>dian'ji</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>su</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>输入_cssid</t>
+    <rPh sb="0" eb="1">
+      <t>shu'ru</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>kw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>sss</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按enter_id</t>
+  </si>
+  <si>
+    <t>kw</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按enter_textname</t>
+    <rPh sb="0" eb="1">
+      <t>an</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>按enter_xpath</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>//*[@id="su"]</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pagedown_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pagedown_xpath</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pagedown_textname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageup_id</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageup_xpath</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>pageup_textname</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ww</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>//*[@id="ww"]</t>
+  </si>
+  <si>
+    <t>word</t>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>No</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>浏览器全屏</t>
+    <rPh sb="0" eb="1">
+      <t>liu'lan'qi</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>quan'p</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>设置分辨率</t>
+    <rPh sb="0" eb="1">
+      <t>she'zhi</t>
+    </rPh>
+    <rPh sb="2" eb="3">
+      <t>fen'bian'l</t>
+    </rPh>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1920,1080</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>123</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -749,7 +908,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -772,8 +931,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -796,8 +960,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="22">
+  <cellStyles count="27">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
     <cellStyle name="超链接" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="超链接" xfId="3" builtinId="8"/>
@@ -820,6 +985,11 @@
     <cellStyle name="已访问的超链接" xfId="19" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="已访问的超链接" xfId="21" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="23" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="25" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="26" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -1097,17 +1267,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="3" width="79" customWidth="1"/>
-    <col min="4" max="4" width="8.83203125" style="1"/>
+    <col min="3" max="3" width="59" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
@@ -1120,7 +1290,7 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
@@ -1258,8 +1428,8 @@
       <c r="C8" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D8" s="9">
-        <v>123</v>
+      <c r="D8" s="9" t="s">
+        <v>152</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
@@ -1267,7 +1437,7 @@
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -1316,7 +1486,7 @@
       <c r="C11" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="9">
         <v>3</v>
       </c>
       <c r="E11" s="1"/>
@@ -1338,14 +1508,14 @@
       <c r="C12" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="9" t="s">
         <v>97</v>
       </c>
       <c r="F12" s="1">
         <v>6</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -1408,7 +1578,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>89</v>
@@ -1425,7 +1595,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>76</v>
@@ -1442,7 +1612,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="8" t="s">
         <v>85</v>
@@ -1459,7 +1629,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>83</v>
@@ -1476,7 +1646,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>89</v>
@@ -1485,7 +1655,7 @@
         <v>4</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1493,7 +1663,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>76</v>
@@ -1510,7 +1680,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C22" s="8" t="s">
         <v>85</v>
@@ -1527,7 +1697,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>83</v>
@@ -1544,7 +1714,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>91</v>
@@ -1561,7 +1731,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C25">
         <v>93</v>
@@ -1570,7 +1740,259 @@
         <v>4</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F26" s="1">
+        <v>6</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C27" t="s">
+        <v>120</v>
+      </c>
+      <c r="F27" s="1">
+        <v>5</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C28" t="s">
+        <v>122</v>
+      </c>
+      <c r="F28" s="1">
+        <v>5</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C29" t="s">
+        <v>126</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="F29" s="1">
+        <v>6</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="C30" t="s">
+        <v>130</v>
+      </c>
+      <c r="F30" s="1">
+        <v>6</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C31" t="s">
+        <v>134</v>
+      </c>
+      <c r="F31" s="1">
+        <v>6</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="1">
+        <v>6</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C33" t="s">
+        <v>143</v>
+      </c>
+      <c r="F33" s="1">
+        <v>6</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C34" t="s">
+        <v>144</v>
+      </c>
+      <c r="F34" s="1">
+        <v>6</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" t="s">
+        <v>145</v>
+      </c>
+      <c r="F35" s="1">
+        <v>6</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C36" t="s">
+        <v>143</v>
+      </c>
+      <c r="F36" s="1">
+        <v>6</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C37" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" s="1">
+        <v>6</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C38" t="s">
+        <v>145</v>
+      </c>
+      <c r="F38" s="1">
+        <v>6</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="F39" s="1">
+        <v>5</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="C40" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="F40" s="1">
+        <v>5</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2199,7 +2621,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>